<commit_message>
conducts S2 and S3 test for traditional GraphQL (resolved fields) and for case with choosen fields
</commit_message>
<xml_diff>
--- a/Wyniki 3/S2 - podsumowanie.xlsx
+++ b/Wyniki 3/S2 - podsumowanie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C1558E-34D9-4E5A-997C-6A8601E7E5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3ADC96-F643-4EA5-A007-207D2B580521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-2340" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="157">
   <si>
     <t>Liczba użytkowników</t>
   </si>
@@ -86,12 +86,6 @@
     <t>REST - jeden endpoint</t>
   </si>
   <si>
-    <t>GraphQL</t>
-  </si>
-  <si>
-    <t>GraphQL - wybrane dane</t>
-  </si>
-  <si>
     <t>2,68ms</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
     <t>293MB</t>
   </si>
   <si>
-    <t>GraphQL - wybrane dane, zoptymalizowane zapytanie do bazy</t>
-  </si>
-  <si>
     <t>1,89ms</t>
   </si>
   <si>
@@ -396,6 +387,126 @@
   </si>
   <si>
     <t>S2 - pobieranie order i order details</t>
+  </si>
+  <si>
+    <t>1.53ms</t>
+  </si>
+  <si>
+    <t>146,81ms</t>
+  </si>
+  <si>
+    <t>4,18ms</t>
+  </si>
+  <si>
+    <t>4,91ms</t>
+  </si>
+  <si>
+    <t>72MB</t>
+  </si>
+  <si>
+    <t>59MB</t>
+  </si>
+  <si>
+    <t>1,95ms</t>
+  </si>
+  <si>
+    <t>144,36ms</t>
+  </si>
+  <si>
+    <t>3,36ms</t>
+  </si>
+  <si>
+    <t>4,14ms</t>
+  </si>
+  <si>
+    <t>721MB</t>
+  </si>
+  <si>
+    <t>591MB</t>
+  </si>
+  <si>
+    <t>1336,67ms</t>
+  </si>
+  <si>
+    <t>1910ms</t>
+  </si>
+  <si>
+    <t>1576,67ms</t>
+  </si>
+  <si>
+    <t>1593,33ms</t>
+  </si>
+  <si>
+    <t>1GB</t>
+  </si>
+  <si>
+    <t>2,37ms</t>
+  </si>
+  <si>
+    <t>148,77ms</t>
+  </si>
+  <si>
+    <t>3,86ms</t>
+  </si>
+  <si>
+    <t>4,51ms</t>
+  </si>
+  <si>
+    <t>49MB</t>
+  </si>
+  <si>
+    <t>40MB</t>
+  </si>
+  <si>
+    <t>1,51ms</t>
+  </si>
+  <si>
+    <t>142,96ms</t>
+  </si>
+  <si>
+    <t>2,57ms</t>
+  </si>
+  <si>
+    <t>3,05ms</t>
+  </si>
+  <si>
+    <t>487MB</t>
+  </si>
+  <si>
+    <t>399MB</t>
+  </si>
+  <si>
+    <t>1163,33ms</t>
+  </si>
+  <si>
+    <t>1760ms</t>
+  </si>
+  <si>
+    <t>1376,67ms</t>
+  </si>
+  <si>
+    <t>1393,33ms</t>
+  </si>
+  <si>
+    <t>899MB</t>
+  </si>
+  <si>
+    <t>738MB</t>
+  </si>
+  <si>
+    <t>GraphQL (jedno zapytanie do bazy, ale nie zoptymalizowane)</t>
+  </si>
+  <si>
+    <t>GraphQL  (jedno zapytanie do bazy, ale nie zoptymalizowane) - wybrane dane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GraphQL (jedno zoptymalizowane zapytanie do bazy) - wybrane dane, </t>
+  </si>
+  <si>
+    <t>Graphql tradycyjny (resolved fields) z data loader i optymalizacją zapytań do bazy</t>
+  </si>
+  <si>
+    <t>Graphql tradycyjny (resolved fields) z data loader i optymalizacją zapytań do bazy, wybrane dane</t>
   </si>
 </sst>
 </file>
@@ -432,7 +543,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -468,11 +579,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -487,6 +609,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -778,32 +903,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G5:P42"/>
+  <dimension ref="G5:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="34.140625" customWidth="1"/>
     <col min="8" max="8" width="53.5703125" customWidth="1"/>
-    <col min="9" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="18" width="13.42578125" customWidth="1"/>
+    <col min="9" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="15" width="18.85546875" customWidth="1"/>
+    <col min="16" max="20" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="7:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="7:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+    </row>
+    <row r="6" spans="7:18" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G6" s="2" t="s">
         <v>0</v>
       </c>
@@ -817,190 +946,244 @@
         <v>15</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G7" s="6">
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G7" s="7">
         <v>100</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G8" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G8" s="7"/>
       <c r="H8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G9" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G9" s="7"/>
       <c r="H9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G10" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G10" s="7"/>
       <c r="H10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G11" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G11" s="7"/>
       <c r="H11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G12" s="6"/>
+      <c r="O11" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G12" s="7"/>
       <c r="H12" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G13" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G13" s="7"/>
       <c r="H13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G14" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G14" s="7"/>
       <c r="H14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G15" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G15" s="7"/>
       <c r="H15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1011,17 +1194,23 @@
         <v>83919</v>
       </c>
       <c r="K15" s="4">
+        <v>84063</v>
+      </c>
+      <c r="L15" s="4">
+        <v>83880.67</v>
+      </c>
+      <c r="M15" s="4">
         <v>83891</v>
       </c>
-      <c r="L15" s="4">
+      <c r="N15" s="4">
         <v>83893</v>
       </c>
-      <c r="M15" s="4">
+      <c r="O15" s="4">
         <v>83902</v>
       </c>
     </row>
-    <row r="16" spans="7:16" x14ac:dyDescent="0.25">
-      <c r="G16" s="6"/>
+    <row r="16" spans="7:18" x14ac:dyDescent="0.25">
+      <c r="G16" s="7"/>
       <c r="H16" s="4" t="s">
         <v>10</v>
       </c>
@@ -1032,229 +1221,287 @@
         <v>87.39</v>
       </c>
       <c r="K16" s="4">
+        <v>87.29</v>
+      </c>
+      <c r="L16" s="4">
+        <v>87.31</v>
+      </c>
+      <c r="M16" s="4">
         <v>87.33</v>
       </c>
-      <c r="L16" s="4">
+      <c r="N16" s="4">
         <v>87.34</v>
       </c>
-      <c r="M16" s="4">
+      <c r="O16" s="4">
         <v>87.36</v>
       </c>
     </row>
-    <row r="17" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G17" s="6"/>
+    <row r="17" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G17" s="7"/>
       <c r="H17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G18" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G18" s="7"/>
       <c r="H18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G19" s="7">
+        <v>70</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G19" s="8">
         <v>1000</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L19" s="5"/>
       <c r="M19" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G20" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G20" s="8"/>
       <c r="H20" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L20" s="5"/>
       <c r="M20" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G21" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G21" s="8"/>
       <c r="H21" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G22" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G22" s="8"/>
       <c r="H22" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L22" s="5"/>
       <c r="M22" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G23" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G23" s="8"/>
       <c r="H23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="I23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="M23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="M23" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G24" s="7"/>
+      <c r="N23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G24" s="8"/>
       <c r="H24" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G25" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G25" s="8"/>
       <c r="H25" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G26" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G26" s="8"/>
       <c r="H26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G27" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G27" s="8"/>
       <c r="H27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1265,17 +1512,23 @@
         <v>839125</v>
       </c>
       <c r="K27" s="5">
+        <v>838605.6</v>
+      </c>
+      <c r="L27" s="5">
+        <v>838984.7</v>
+      </c>
+      <c r="M27" s="5">
         <v>838797</v>
       </c>
-      <c r="L27" s="5">
+      <c r="N27" s="5">
         <v>838682</v>
       </c>
-      <c r="M27" s="5">
+      <c r="O27" s="5">
         <v>838856</v>
       </c>
     </row>
-    <row r="28" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G28" s="7"/>
+    <row r="28" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G28" s="8"/>
       <c r="H28" s="5" t="s">
         <v>10</v>
       </c>
@@ -1286,229 +1539,287 @@
         <v>873.37</v>
       </c>
       <c r="K28" s="5">
+        <v>873.06</v>
+      </c>
+      <c r="L28" s="5">
+        <v>873.14</v>
+      </c>
+      <c r="M28" s="5">
         <v>873.25</v>
       </c>
-      <c r="L28" s="5">
+      <c r="N28" s="5">
         <v>873.19</v>
       </c>
-      <c r="M28" s="5">
+      <c r="O28" s="5">
         <v>873.1</v>
       </c>
     </row>
-    <row r="29" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G29" s="7"/>
+    <row r="29" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G29" s="8"/>
       <c r="H29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G30" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G30" s="8"/>
       <c r="H30" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>78</v>
+        <v>128</v>
       </c>
       <c r="L30" s="5" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G31" s="6">
+        <v>75</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G31" s="7">
         <v>4000</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>1</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L31" s="4"/>
       <c r="M31" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G32" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G32" s="7"/>
       <c r="H32" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L32" s="4"/>
       <c r="M32" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G33" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G33" s="7"/>
       <c r="H33" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L33" s="4"/>
       <c r="M33" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G34" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G34" s="7"/>
       <c r="H34" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G35" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G35" s="7"/>
       <c r="H35" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>79</v>
+        <v>59</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>96</v>
+        <v>146</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G36" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G36" s="7"/>
       <c r="H36" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G37" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G37" s="7"/>
       <c r="H37" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G38" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G38" s="7"/>
       <c r="H38" s="4" t="s">
         <v>8</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G39" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G39" s="7"/>
       <c r="H39" s="4" t="s">
         <v>9</v>
       </c>
@@ -1519,17 +1830,23 @@
         <v>2127163</v>
       </c>
       <c r="K39" s="4">
+        <v>1435061.67</v>
+      </c>
+      <c r="L39" s="4">
+        <v>1551003</v>
+      </c>
+      <c r="M39" s="4">
         <v>1641889.4</v>
       </c>
-      <c r="L39" s="4">
+      <c r="N39" s="4">
         <v>1693267</v>
       </c>
-      <c r="M39" s="4">
+      <c r="O39" s="4">
         <v>1860542</v>
       </c>
     </row>
-    <row r="40" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G40" s="6"/>
+    <row r="40" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G40" s="7"/>
       <c r="H40" s="4" t="s">
         <v>10</v>
       </c>
@@ -1540,55 +1857,73 @@
         <v>2214.0700000000002</v>
       </c>
       <c r="K40" s="4">
+        <v>1493.66</v>
+      </c>
+      <c r="L40" s="4">
+        <v>1614.5</v>
+      </c>
+      <c r="M40" s="4">
         <v>1708.95</v>
       </c>
-      <c r="L40" s="4">
+      <c r="N40" s="4">
         <v>1762.45</v>
       </c>
-      <c r="M40" s="4">
+      <c r="O40" s="4">
         <v>1936.596</v>
       </c>
     </row>
-    <row r="41" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G41" s="6"/>
+    <row r="41" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G41" s="7"/>
       <c r="H41" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G42" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G42" s="7"/>
       <c r="H42" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>118</v>
+        <v>81</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1596,7 +1931,7 @@
     <mergeCell ref="G7:G18"/>
     <mergeCell ref="G19:G30"/>
     <mergeCell ref="G31:G42"/>
-    <mergeCell ref="G5:M5"/>
+    <mergeCell ref="G5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>